<commit_message>
create data sensitive summaries for G3
</commit_message>
<xml_diff>
--- a/Analyses/main study - LLM/create tables, graphics G3/outputs/RR_codes_complete.xlsx
+++ b/Analyses/main study - LLM/create tables, graphics G3/outputs/RR_codes_complete.xlsx
@@ -414,7 +414,7 @@
         <v>0</v>
       </c>
       <c r="F2">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3">
@@ -466,6 +466,12 @@
           <t>Identifies instances where participants express discomfort or unease towards rescue robots due to their human-like characteristics, including their imitation of nature, intimidating appearance, and how these traits might evoke feelings of unease.</t>
         </is>
       </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4">
+        <v>3</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -492,7 +498,7 @@
         <v>0</v>
       </c>
       <c r="F5">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6">
@@ -520,7 +526,7 @@
         <v>1</v>
       </c>
       <c r="F6">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7">
@@ -548,7 +554,7 @@
         <v>0</v>
       </c>
       <c r="F7">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8">
@@ -576,7 +582,7 @@
         <v>0</v>
       </c>
       <c r="F8">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="9">
@@ -632,7 +638,7 @@
         <v>0</v>
       </c>
       <c r="F10">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="11">
@@ -679,7 +685,7 @@
         </is>
       </c>
       <c r="E12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F12">
         <v>7</v>
@@ -707,10 +713,10 @@
         </is>
       </c>
       <c r="E13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F13">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="14">
@@ -735,7 +741,7 @@
         </is>
       </c>
       <c r="E14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F14">
         <v>4</v>
@@ -763,10 +769,10 @@
         </is>
       </c>
       <c r="E15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F15">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="16">
@@ -790,6 +796,12 @@
           <t>Highlights physical and mental stamina in Human-Robot-Interaction, focusing on the importance of sustaining performance and functionality during prolonged rescue operations, without unnecessary details or quotes.</t>
         </is>
       </c>
+      <c r="E16">
+        <v>1</v>
+      </c>
+      <c r="F16">
+        <v>1</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -869,10 +881,10 @@
         </is>
       </c>
       <c r="E19">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F19">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="20">
@@ -897,10 +909,10 @@
         </is>
       </c>
       <c r="E20">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F20">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="21">
@@ -925,7 +937,7 @@
         </is>
       </c>
       <c r="E21">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F21">
         <v>8</v>
@@ -956,7 +968,7 @@
         <v>10</v>
       </c>
       <c r="F22">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="23">
@@ -984,7 +996,7 @@
         <v>1</v>
       </c>
       <c r="F23">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24">
@@ -1009,10 +1021,10 @@
         </is>
       </c>
       <c r="E24">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F24">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="25">
@@ -1037,10 +1049,10 @@
         </is>
       </c>
       <c r="E25">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F25">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="26">
@@ -1065,10 +1077,10 @@
         </is>
       </c>
       <c r="E26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F26">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="27">
@@ -1092,12 +1104,6 @@
           <t>Identifies concerns expressed about the susceptibility of rescue robots to hacking, emphasizing identifiable, factual dangers or vulnerabilities that could occur in real-world scenarios.</t>
         </is>
       </c>
-      <c r="E27">
-        <v>1</v>
-      </c>
-      <c r="F27">
-        <v>1</v>
-      </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -1124,7 +1130,7 @@
         <v>0</v>
       </c>
       <c r="F28">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="29">
@@ -1149,7 +1155,7 @@
         </is>
       </c>
       <c r="E29">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="F29">
         <v>1</v>
@@ -1177,10 +1183,10 @@
         </is>
       </c>
       <c r="E30">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F30">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="31">
@@ -1205,10 +1211,10 @@
         </is>
       </c>
       <c r="E31">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F31">
-        <v>31</v>
+        <v>23</v>
       </c>
     </row>
     <row r="32">
@@ -1233,10 +1239,10 @@
         </is>
       </c>
       <c r="E32">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F32">
-        <v>11</v>
+        <v>15</v>
       </c>
     </row>
     <row r="33">
@@ -1289,7 +1295,7 @@
         </is>
       </c>
       <c r="E34">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="F34">
         <v>20</v>
@@ -1317,10 +1323,10 @@
         </is>
       </c>
       <c r="E35">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F35">
-        <v>11</v>
+        <v>14</v>
       </c>
     </row>
     <row r="36">
@@ -1345,10 +1351,10 @@
         </is>
       </c>
       <c r="E36">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F36">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="37">
@@ -1373,10 +1379,10 @@
         </is>
       </c>
       <c r="E37">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F37">
-        <v>12</v>
+        <v>15</v>
       </c>
     </row>
     <row r="38">
@@ -1401,10 +1407,10 @@
         </is>
       </c>
       <c r="E38">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F38">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="39">
@@ -1429,7 +1435,7 @@
         </is>
       </c>
       <c r="E39">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="F39">
         <v>22</v>
@@ -1457,10 +1463,10 @@
         </is>
       </c>
       <c r="E40">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F40">
-        <v>21</v>
+        <v>30</v>
       </c>
     </row>
     <row r="41">
@@ -1488,7 +1494,7 @@
         <v>6</v>
       </c>
       <c r="F41">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="42">
@@ -1541,7 +1547,7 @@
         </is>
       </c>
       <c r="E43">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F43">
         <v>1</v>
@@ -1572,7 +1578,7 @@
         <v>2</v>
       </c>
       <c r="F44">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="45">
@@ -1596,12 +1602,6 @@
           <t>Identifies concerns and questions related to potential delays in the operational capabilities of rescue robots, particularly focusing on issues such as battery life, recharging times, and energy management.</t>
         </is>
       </c>
-      <c r="E45">
-        <v>0</v>
-      </c>
-      <c r="F45">
-        <v>2</v>
-      </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
@@ -1628,7 +1628,7 @@
         <v>0</v>
       </c>
       <c r="F46">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="47">
@@ -1653,10 +1653,10 @@
         </is>
       </c>
       <c r="E47">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="F47">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="48">
@@ -1681,10 +1681,10 @@
         </is>
       </c>
       <c r="E48">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F48">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="49">
@@ -1709,10 +1709,10 @@
         </is>
       </c>
       <c r="E49">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F49">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="50">
@@ -1762,7 +1762,7 @@
         <v>2</v>
       </c>
       <c r="F51">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="52">
@@ -1787,10 +1787,10 @@
         </is>
       </c>
       <c r="E52">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F52">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="53">
@@ -1818,7 +1818,7 @@
         <v>0</v>
       </c>
       <c r="F53">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="54">
@@ -1843,10 +1843,10 @@
         </is>
       </c>
       <c r="E54">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="F54">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="55">
@@ -1871,10 +1871,10 @@
         </is>
       </c>
       <c r="E55">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F55">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="56">
@@ -1927,7 +1927,7 @@
         </is>
       </c>
       <c r="E57">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F57">
         <v>2</v>
@@ -1983,7 +1983,7 @@
         </is>
       </c>
       <c r="E59">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F59">
         <v>2</v>
@@ -2011,10 +2011,10 @@
         </is>
       </c>
       <c r="E60">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F60">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="61">
@@ -2039,10 +2039,10 @@
         </is>
       </c>
       <c r="E61">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F61">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="62">
@@ -2067,10 +2067,10 @@
         </is>
       </c>
       <c r="E62">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F62">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="63">
@@ -2095,7 +2095,7 @@
         </is>
       </c>
       <c r="E63">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F63">
         <v>5</v>
@@ -2123,10 +2123,10 @@
         </is>
       </c>
       <c r="E64">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="F64">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="65">
@@ -2151,10 +2151,10 @@
         </is>
       </c>
       <c r="E65">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F65">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="66">
@@ -2179,7 +2179,7 @@
         </is>
       </c>
       <c r="E66">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F66">
         <v>3</v>
@@ -2207,10 +2207,10 @@
         </is>
       </c>
       <c r="E67">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F67">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="68">
@@ -2235,10 +2235,10 @@
         </is>
       </c>
       <c r="E68">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F68">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="69">
@@ -2263,10 +2263,10 @@
         </is>
       </c>
       <c r="E69">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F69">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="70">
@@ -2294,7 +2294,7 @@
         <v>1</v>
       </c>
       <c r="F70">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="71">
@@ -2319,10 +2319,10 @@
         </is>
       </c>
       <c r="E71">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F71">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="72">
@@ -2347,10 +2347,10 @@
         </is>
       </c>
       <c r="E72">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F72">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="73">
@@ -2375,10 +2375,10 @@
         </is>
       </c>
       <c r="E73">
+        <v>1</v>
+      </c>
+      <c r="F73">
         <v>2</v>
-      </c>
-      <c r="F73">
-        <v>3</v>
       </c>
     </row>
     <row r="74">
@@ -2403,7 +2403,7 @@
         </is>
       </c>
       <c r="E74">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F74">
         <v>2</v>
@@ -2431,10 +2431,10 @@
         </is>
       </c>
       <c r="E75">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F75">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="76">
@@ -2459,10 +2459,10 @@
         </is>
       </c>
       <c r="E76">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F76">
-        <v>7</v>
+        <v>12</v>
       </c>
     </row>
     <row r="77">
@@ -2487,10 +2487,10 @@
         </is>
       </c>
       <c r="E77">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F77">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="78">
@@ -2515,10 +2515,10 @@
         </is>
       </c>
       <c r="E78">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F78">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="79">
@@ -2543,10 +2543,10 @@
         </is>
       </c>
       <c r="E79">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F79">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="80">
@@ -2571,7 +2571,7 @@
         </is>
       </c>
       <c r="E80">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F80">
         <v>4</v>
@@ -2599,10 +2599,10 @@
         </is>
       </c>
       <c r="E81">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F81">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="82">
@@ -2630,7 +2630,7 @@
         <v>1</v>
       </c>
       <c r="F82">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="83">
@@ -2655,10 +2655,10 @@
         </is>
       </c>
       <c r="E83">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F83">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="84">
@@ -2683,10 +2683,10 @@
         </is>
       </c>
       <c r="E84">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F84">
-        <v>16</v>
+        <v>22</v>
       </c>
     </row>
     <row r="85">
@@ -2711,10 +2711,10 @@
         </is>
       </c>
       <c r="E85">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F85">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="86">
@@ -2739,10 +2739,10 @@
         </is>
       </c>
       <c r="E86">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F86">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="87">
@@ -2767,7 +2767,7 @@
         </is>
       </c>
       <c r="E87">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F87">
         <v>6</v>
@@ -2795,7 +2795,7 @@
         </is>
       </c>
       <c r="E88">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F88">
         <v>2</v>
@@ -2823,10 +2823,10 @@
         </is>
       </c>
       <c r="E89">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F89">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="90">
@@ -2851,10 +2851,10 @@
         </is>
       </c>
       <c r="E90">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F90">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="91">
@@ -2879,10 +2879,10 @@
         </is>
       </c>
       <c r="E91">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F91">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
new layout G3 graphics
</commit_message>
<xml_diff>
--- a/Analyses/main study - LLM/create tables, graphics G3/outputs/RR_codes_complete.xlsx
+++ b/Analyses/main study - LLM/create tables, graphics G3/outputs/RR_codes_complete.xlsx
@@ -380,12 +380,12 @@
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
+          <t>rigid</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
           <t>soft</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>rigid</t>
         </is>
       </c>
     </row>
@@ -411,10 +411,10 @@
         </is>
       </c>
       <c r="E2">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="F2">
-        <v>8</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3">
@@ -439,10 +439,10 @@
         </is>
       </c>
       <c r="E3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F3">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4">
@@ -467,10 +467,10 @@
         </is>
       </c>
       <c r="E4">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F4">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5">
@@ -495,10 +495,10 @@
         </is>
       </c>
       <c r="E5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6">
@@ -523,10 +523,10 @@
         </is>
       </c>
       <c r="E6">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F6">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7">
@@ -551,10 +551,10 @@
         </is>
       </c>
       <c r="E7">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F7">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8">
@@ -579,10 +579,10 @@
         </is>
       </c>
       <c r="E8">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F8">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9">
@@ -607,10 +607,10 @@
         </is>
       </c>
       <c r="E9">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F9">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10">
@@ -635,10 +635,10 @@
         </is>
       </c>
       <c r="E10">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="F10">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11">
@@ -685,10 +685,10 @@
         </is>
       </c>
       <c r="E12">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F12">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13">
@@ -713,10 +713,10 @@
         </is>
       </c>
       <c r="E13">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F13">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14">
@@ -741,10 +741,10 @@
         </is>
       </c>
       <c r="E14">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F14">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15">
@@ -769,10 +769,10 @@
         </is>
       </c>
       <c r="E15">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="F15">
-        <v>7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16">
@@ -881,10 +881,10 @@
         </is>
       </c>
       <c r="E19">
+        <v>3</v>
+      </c>
+      <c r="F19">
         <v>18</v>
-      </c>
-      <c r="F19">
-        <v>3</v>
       </c>
     </row>
     <row r="20">
@@ -909,10 +909,10 @@
         </is>
       </c>
       <c r="E20">
+        <v>8</v>
+      </c>
+      <c r="F20">
         <v>3</v>
-      </c>
-      <c r="F20">
-        <v>8</v>
       </c>
     </row>
     <row r="21">
@@ -937,10 +937,10 @@
         </is>
       </c>
       <c r="E21">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="F21">
-        <v>8</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22">
@@ -965,10 +965,10 @@
         </is>
       </c>
       <c r="E22">
+        <v>7</v>
+      </c>
+      <c r="F22">
         <v>10</v>
-      </c>
-      <c r="F22">
-        <v>7</v>
       </c>
     </row>
     <row r="23">
@@ -1021,10 +1021,10 @@
         </is>
       </c>
       <c r="E24">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="F24">
-        <v>8</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25">
@@ -1049,10 +1049,10 @@
         </is>
       </c>
       <c r="E25">
+        <v>11</v>
+      </c>
+      <c r="F25">
         <v>2</v>
-      </c>
-      <c r="F25">
-        <v>11</v>
       </c>
     </row>
     <row r="26">
@@ -1077,10 +1077,10 @@
         </is>
       </c>
       <c r="E26">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F26">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="27">
@@ -1127,10 +1127,10 @@
         </is>
       </c>
       <c r="E28">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F28">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="29">
@@ -1155,10 +1155,10 @@
         </is>
       </c>
       <c r="E29">
+        <v>1</v>
+      </c>
+      <c r="F29">
         <v>9</v>
-      </c>
-      <c r="F29">
-        <v>1</v>
       </c>
     </row>
     <row r="30">
@@ -1183,10 +1183,10 @@
         </is>
       </c>
       <c r="E30">
+        <v>17</v>
+      </c>
+      <c r="F30">
         <v>2</v>
-      </c>
-      <c r="F30">
-        <v>17</v>
       </c>
     </row>
     <row r="31">
@@ -1211,10 +1211,10 @@
         </is>
       </c>
       <c r="E31">
+        <v>23</v>
+      </c>
+      <c r="F31">
         <v>6</v>
-      </c>
-      <c r="F31">
-        <v>23</v>
       </c>
     </row>
     <row r="32">
@@ -1239,10 +1239,10 @@
         </is>
       </c>
       <c r="E32">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="F32">
-        <v>15</v>
+        <v>1</v>
       </c>
     </row>
     <row r="33">
@@ -1267,10 +1267,10 @@
         </is>
       </c>
       <c r="E33">
+        <v>30</v>
+      </c>
+      <c r="F33">
         <v>2</v>
-      </c>
-      <c r="F33">
-        <v>30</v>
       </c>
     </row>
     <row r="34">
@@ -1295,10 +1295,10 @@
         </is>
       </c>
       <c r="E34">
+        <v>20</v>
+      </c>
+      <c r="F34">
         <v>6</v>
-      </c>
-      <c r="F34">
-        <v>20</v>
       </c>
     </row>
     <row r="35">
@@ -1323,10 +1323,10 @@
         </is>
       </c>
       <c r="E35">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="F35">
-        <v>14</v>
+        <v>0</v>
       </c>
     </row>
     <row r="36">
@@ -1351,10 +1351,10 @@
         </is>
       </c>
       <c r="E36">
+        <v>10</v>
+      </c>
+      <c r="F36">
         <v>3</v>
-      </c>
-      <c r="F36">
-        <v>10</v>
       </c>
     </row>
     <row r="37">
@@ -1379,10 +1379,10 @@
         </is>
       </c>
       <c r="E37">
+        <v>15</v>
+      </c>
+      <c r="F37">
         <v>2</v>
-      </c>
-      <c r="F37">
-        <v>15</v>
       </c>
     </row>
     <row r="38">
@@ -1407,10 +1407,10 @@
         </is>
       </c>
       <c r="E38">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="F38">
-        <v>12</v>
+        <v>1</v>
       </c>
     </row>
     <row r="39">
@@ -1435,10 +1435,10 @@
         </is>
       </c>
       <c r="E39">
+        <v>22</v>
+      </c>
+      <c r="F39">
         <v>6</v>
-      </c>
-      <c r="F39">
-        <v>22</v>
       </c>
     </row>
     <row r="40">
@@ -1463,10 +1463,10 @@
         </is>
       </c>
       <c r="E40">
+        <v>30</v>
+      </c>
+      <c r="F40">
         <v>4</v>
-      </c>
-      <c r="F40">
-        <v>30</v>
       </c>
     </row>
     <row r="41">
@@ -1491,10 +1491,10 @@
         </is>
       </c>
       <c r="E41">
+        <v>8</v>
+      </c>
+      <c r="F41">
         <v>6</v>
-      </c>
-      <c r="F41">
-        <v>8</v>
       </c>
     </row>
     <row r="42">
@@ -1519,10 +1519,10 @@
         </is>
       </c>
       <c r="E42">
+        <v>23</v>
+      </c>
+      <c r="F42">
         <v>2</v>
-      </c>
-      <c r="F42">
-        <v>23</v>
       </c>
     </row>
     <row r="43">
@@ -1547,10 +1547,10 @@
         </is>
       </c>
       <c r="E43">
+        <v>1</v>
+      </c>
+      <c r="F43">
         <v>2</v>
-      </c>
-      <c r="F43">
-        <v>1</v>
       </c>
     </row>
     <row r="44">
@@ -1625,10 +1625,10 @@
         </is>
       </c>
       <c r="E46">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F46">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="47">
@@ -1653,10 +1653,10 @@
         </is>
       </c>
       <c r="E47">
+        <v>13</v>
+      </c>
+      <c r="F47">
         <v>4</v>
-      </c>
-      <c r="F47">
-        <v>13</v>
       </c>
     </row>
     <row r="48">
@@ -1681,10 +1681,10 @@
         </is>
       </c>
       <c r="E48">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F48">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="49">
@@ -1709,10 +1709,10 @@
         </is>
       </c>
       <c r="E49">
+        <v>7</v>
+      </c>
+      <c r="F49">
         <v>2</v>
-      </c>
-      <c r="F49">
-        <v>7</v>
       </c>
     </row>
     <row r="50">
@@ -1759,10 +1759,10 @@
         </is>
       </c>
       <c r="E51">
+        <v>7</v>
+      </c>
+      <c r="F51">
         <v>2</v>
-      </c>
-      <c r="F51">
-        <v>7</v>
       </c>
     </row>
     <row r="52">
@@ -1787,10 +1787,10 @@
         </is>
       </c>
       <c r="E52">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="F52">
-        <v>12</v>
+        <v>1</v>
       </c>
     </row>
     <row r="53">
@@ -1815,10 +1815,10 @@
         </is>
       </c>
       <c r="E53">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F53">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="54">
@@ -1843,10 +1843,10 @@
         </is>
       </c>
       <c r="E54">
+        <v>2</v>
+      </c>
+      <c r="F54">
         <v>16</v>
-      </c>
-      <c r="F54">
-        <v>2</v>
       </c>
     </row>
     <row r="55">
@@ -1871,10 +1871,10 @@
         </is>
       </c>
       <c r="E55">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="F55">
-        <v>9</v>
+        <v>0</v>
       </c>
     </row>
     <row r="56">
@@ -1899,10 +1899,10 @@
         </is>
       </c>
       <c r="E56">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F56">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="57">
@@ -1927,10 +1927,10 @@
         </is>
       </c>
       <c r="E57">
+        <v>2</v>
+      </c>
+      <c r="F57">
         <v>3</v>
-      </c>
-      <c r="F57">
-        <v>2</v>
       </c>
     </row>
     <row r="58">
@@ -1955,10 +1955,10 @@
         </is>
       </c>
       <c r="E58">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F58">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="59">
@@ -1983,10 +1983,10 @@
         </is>
       </c>
       <c r="E59">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F59">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="60">
@@ -2011,10 +2011,10 @@
         </is>
       </c>
       <c r="E60">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="F60">
-        <v>6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="61">
@@ -2039,10 +2039,10 @@
         </is>
       </c>
       <c r="E61">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="F61">
-        <v>11</v>
+        <v>0</v>
       </c>
     </row>
     <row r="62">
@@ -2067,10 +2067,10 @@
         </is>
       </c>
       <c r="E62">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F62">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="63">
@@ -2095,10 +2095,10 @@
         </is>
       </c>
       <c r="E63">
+        <v>5</v>
+      </c>
+      <c r="F63">
         <v>2</v>
-      </c>
-      <c r="F63">
-        <v>5</v>
       </c>
     </row>
     <row r="64">
@@ -2123,10 +2123,10 @@
         </is>
       </c>
       <c r="E64">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="F64">
-        <v>9</v>
+        <v>1</v>
       </c>
     </row>
     <row r="65">
@@ -2151,10 +2151,10 @@
         </is>
       </c>
       <c r="E65">
+        <v>7</v>
+      </c>
+      <c r="F65">
         <v>2</v>
-      </c>
-      <c r="F65">
-        <v>7</v>
       </c>
     </row>
     <row r="66">
@@ -2179,10 +2179,10 @@
         </is>
       </c>
       <c r="E66">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F66">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="67">
@@ -2207,10 +2207,10 @@
         </is>
       </c>
       <c r="E67">
+        <v>8</v>
+      </c>
+      <c r="F67">
         <v>24</v>
-      </c>
-      <c r="F67">
-        <v>8</v>
       </c>
     </row>
     <row r="68">
@@ -2235,10 +2235,10 @@
         </is>
       </c>
       <c r="E68">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="F68">
-        <v>9</v>
+        <v>1</v>
       </c>
     </row>
     <row r="69">
@@ -2263,10 +2263,10 @@
         </is>
       </c>
       <c r="E69">
+        <v>10</v>
+      </c>
+      <c r="F69">
         <v>3</v>
-      </c>
-      <c r="F69">
-        <v>10</v>
       </c>
     </row>
     <row r="70">
@@ -2291,10 +2291,10 @@
         </is>
       </c>
       <c r="E70">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F70">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="71">
@@ -2319,10 +2319,10 @@
         </is>
       </c>
       <c r="E71">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="F71">
-        <v>7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="72">
@@ -2347,10 +2347,10 @@
         </is>
       </c>
       <c r="E72">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="F72">
-        <v>11</v>
+        <v>1</v>
       </c>
     </row>
     <row r="73">
@@ -2375,10 +2375,10 @@
         </is>
       </c>
       <c r="E73">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F73">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="74">
@@ -2403,10 +2403,10 @@
         </is>
       </c>
       <c r="E74">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F74">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="75">
@@ -2431,10 +2431,10 @@
         </is>
       </c>
       <c r="E75">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F75">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="76">
@@ -2459,10 +2459,10 @@
         </is>
       </c>
       <c r="E76">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="F76">
-        <v>12</v>
+        <v>1</v>
       </c>
     </row>
     <row r="77">
@@ -2515,10 +2515,10 @@
         </is>
       </c>
       <c r="E78">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="F78">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="79">
@@ -2543,10 +2543,10 @@
         </is>
       </c>
       <c r="E79">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="F79">
-        <v>8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="80">
@@ -2571,10 +2571,10 @@
         </is>
       </c>
       <c r="E80">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F80">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="81">
@@ -2599,10 +2599,10 @@
         </is>
       </c>
       <c r="E81">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="F81">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="82">
@@ -2627,10 +2627,10 @@
         </is>
       </c>
       <c r="E82">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F82">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="83">
@@ -2655,10 +2655,10 @@
         </is>
       </c>
       <c r="E83">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F83">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="84">
@@ -2683,10 +2683,10 @@
         </is>
       </c>
       <c r="E84">
+        <v>22</v>
+      </c>
+      <c r="F84">
         <v>7</v>
-      </c>
-      <c r="F84">
-        <v>22</v>
       </c>
     </row>
     <row r="85">
@@ -2711,10 +2711,10 @@
         </is>
       </c>
       <c r="E85">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F85">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="86">
@@ -2739,10 +2739,10 @@
         </is>
       </c>
       <c r="E86">
+        <v>5</v>
+      </c>
+      <c r="F86">
         <v>2</v>
-      </c>
-      <c r="F86">
-        <v>5</v>
       </c>
     </row>
     <row r="87">
@@ -2767,10 +2767,10 @@
         </is>
       </c>
       <c r="E87">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="F87">
-        <v>6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="88">
@@ -2823,10 +2823,10 @@
         </is>
       </c>
       <c r="E89">
+        <v>8</v>
+      </c>
+      <c r="F89">
         <v>3</v>
-      </c>
-      <c r="F89">
-        <v>8</v>
       </c>
     </row>
     <row r="90">
@@ -2851,10 +2851,10 @@
         </is>
       </c>
       <c r="E90">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F90">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="91">
@@ -2879,10 +2879,10 @@
         </is>
       </c>
       <c r="E91">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F91">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>